<commit_message>
Update documents for 2018-06-05 call with UCB
</commit_message>
<xml_diff>
--- a/docs/Report/tables.xlsx
+++ b/docs/Report/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="prevalenceAS" sheetId="1" r:id="rId1"/>
@@ -3518,8 +3518,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -4002,14 +4002,14 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -4068,44 +4068,19 @@
   </cellStyles>
   <dxfs count="53">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4189,25 +4164,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4217,19 +4198,38 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -4246,15 +4246,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A1:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="year" dataDxfId="45"/>
-    <tableColumn id="2" name="numer5pct" dataDxfId="46" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="denom5pct" dataDxfId="52" dataCellStyle="Comma"/>
-    <tableColumn id="4" name="numerEstimated" dataDxfId="51" dataCellStyle="Comma"/>
-    <tableColumn id="5" name="denomEstimated" dataDxfId="50" dataCellStyle="Comma"/>
-    <tableColumn id="6" name="prev" dataDxfId="49" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="year" dataDxfId="50"/>
+    <tableColumn id="2" name="numer5pct" dataDxfId="49" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="denom5pct" dataDxfId="48" dataCellStyle="Comma"/>
+    <tableColumn id="4" name="numerEstimated" dataDxfId="47" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="denomEstimated" dataDxfId="46" dataCellStyle="Comma"/>
+    <tableColumn id="6" name="prev" dataDxfId="45" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4266,23 +4266,23 @@
   <tableColumns count="5">
     <tableColumn id="1" name="cohort"/>
     <tableColumn id="2" name="database"/>
-    <tableColumn id="3" name="denom" dataDxfId="12"/>
-    <tableColumn id="4" name="age" dataDxfId="11"/>
-    <tableColumn id="5" name="female" dataDxfId="10"/>
+    <tableColumn id="3" name="denom" dataDxfId="44"/>
+    <tableColumn id="4" name="age" dataDxfId="43"/>
+    <tableColumn id="5" name="female" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="G1:K6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="G1:K6" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="G1:K6"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="cohort" dataDxfId="6"/>
-    <tableColumn id="2" name="database" dataDxfId="5"/>
-    <tableColumn id="3" name="denom" dataDxfId="3"/>
-    <tableColumn id="4" name="age" dataDxfId="4"/>
-    <tableColumn id="5" name="female" dataDxfId="9"/>
+    <tableColumn id="1" name="cohort" dataDxfId="39"/>
+    <tableColumn id="2" name="database" dataDxfId="38"/>
+    <tableColumn id="3" name="denom" dataDxfId="37"/>
+    <tableColumn id="4" name="age" dataDxfId="36"/>
+    <tableColumn id="5" name="female" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4294,9 +4294,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="database"/>
     <tableColumn id="2" name="exposure"/>
-    <tableColumn id="3" name="denom" dataDxfId="2"/>
-    <tableColumn id="4" name="age" dataDxfId="1"/>
-    <tableColumn id="5" name="female" dataDxfId="0"/>
+    <tableColumn id="3" name="denom" dataDxfId="34"/>
+    <tableColumn id="4" name="age" dataDxfId="33"/>
+    <tableColumn id="5" name="female" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4315,9 +4315,9 @@
     <tableColumn id="1" name="outcomeCategory"/>
     <tableColumn id="2" name="disease"/>
     <tableColumn id="3" name="timeWindow"/>
-    <tableColumn id="4" name="MPCD AS cohort" dataDxfId="27"/>
-    <tableColumn id="5" name="Marketscan AS cohort" dataDxfId="26"/>
-    <tableColumn id="6" name="Medicare AS cohort" dataDxfId="25"/>
+    <tableColumn id="4" name="MPCD AS cohort" dataDxfId="31"/>
+    <tableColumn id="5" name="Marketscan AS cohort" dataDxfId="30"/>
+    <tableColumn id="6" name="Medicare AS cohort" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4336,18 +4336,18 @@
     <tableColumn id="1" name="outcomeCategory"/>
     <tableColumn id="2" name="disease"/>
     <tableColumn id="3" name="timeWindow"/>
-    <tableColumn id="4" name="MPCD TNF" dataDxfId="39"/>
-    <tableColumn id="5" name="MPCD DMARD" dataDxfId="38"/>
-    <tableColumn id="6" name="MPCD NSAID" dataDxfId="37"/>
-    <tableColumn id="7" name="MPCD No exposure" dataDxfId="36"/>
-    <tableColumn id="8" name="Marketscan TNF" dataDxfId="35"/>
-    <tableColumn id="9" name="Marketscan DMARD" dataDxfId="34"/>
-    <tableColumn id="10" name="Marketscan NSAID" dataDxfId="33"/>
-    <tableColumn id="11" name="Marketscan No exposure" dataDxfId="32"/>
-    <tableColumn id="12" name="Medicare TNF" dataDxfId="31"/>
-    <tableColumn id="13" name="Medicare DMARD" dataDxfId="30"/>
-    <tableColumn id="14" name="Medicare NSAID" dataDxfId="29"/>
-    <tableColumn id="15" name="Medicare No exposure" dataDxfId="28"/>
+    <tableColumn id="4" name="MPCD TNF" dataDxfId="28"/>
+    <tableColumn id="5" name="MPCD DMARD" dataDxfId="27"/>
+    <tableColumn id="6" name="MPCD NSAID" dataDxfId="26"/>
+    <tableColumn id="7" name="MPCD No exposure" dataDxfId="25"/>
+    <tableColumn id="8" name="Marketscan TNF" dataDxfId="24"/>
+    <tableColumn id="9" name="Marketscan DMARD" dataDxfId="23"/>
+    <tableColumn id="10" name="Marketscan NSAID" dataDxfId="22"/>
+    <tableColumn id="11" name="Marketscan No exposure" dataDxfId="21"/>
+    <tableColumn id="12" name="Medicare TNF" dataDxfId="20"/>
+    <tableColumn id="13" name="Medicare DMARD" dataDxfId="19"/>
+    <tableColumn id="14" name="Medicare NSAID" dataDxfId="18"/>
+    <tableColumn id="15" name="Medicare No exposure" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4360,18 +4360,18 @@
     <tableColumn id="1" name="type"/>
     <tableColumn id="2" name="outcomeCategory"/>
     <tableColumn id="3" name="disease"/>
-    <tableColumn id="4" name="MPCD TNF" dataDxfId="24"/>
-    <tableColumn id="5" name="MPCD DMARD" dataDxfId="23"/>
-    <tableColumn id="6" name="MPCD NSAID" dataDxfId="22"/>
-    <tableColumn id="7" name="MPCD No exposure" dataDxfId="21"/>
-    <tableColumn id="8" name="Marketscan TNF" dataDxfId="20"/>
-    <tableColumn id="9" name="Marketscan DMARD" dataDxfId="19"/>
-    <tableColumn id="10" name="Marketscan NSAID" dataDxfId="18"/>
-    <tableColumn id="11" name="Marketscan No exposure" dataDxfId="17"/>
-    <tableColumn id="12" name="Medicare TNF" dataDxfId="16"/>
-    <tableColumn id="13" name="Medicare DMARD" dataDxfId="15"/>
-    <tableColumn id="14" name="Medicare NSAID" dataDxfId="14"/>
-    <tableColumn id="15" name="Medicare No exposure" dataDxfId="13"/>
+    <tableColumn id="4" name="MPCD TNF" dataDxfId="16"/>
+    <tableColumn id="5" name="MPCD DMARD" dataDxfId="15"/>
+    <tableColumn id="6" name="MPCD NSAID" dataDxfId="14"/>
+    <tableColumn id="7" name="MPCD No exposure" dataDxfId="13"/>
+    <tableColumn id="8" name="Marketscan TNF" dataDxfId="12"/>
+    <tableColumn id="9" name="Marketscan DMARD" dataDxfId="11"/>
+    <tableColumn id="10" name="Marketscan NSAID" dataDxfId="10"/>
+    <tableColumn id="11" name="Marketscan No exposure" dataDxfId="9"/>
+    <tableColumn id="12" name="Medicare TNF" dataDxfId="8"/>
+    <tableColumn id="13" name="Medicare DMARD" dataDxfId="7"/>
+    <tableColumn id="14" name="Medicare NSAID" dataDxfId="6"/>
+    <tableColumn id="15" name="Medicare No exposure" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4397,11 +4397,11 @@
     <tableColumn id="3" name="model"/>
     <tableColumn id="4" name="comparison"/>
     <tableColumn id="5" name="database"/>
-    <tableColumn id="6" name="nTNF" dataDxfId="42" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="nComparator" dataDxfId="40" dataCellStyle="Comma"/>
-    <tableColumn id="8" name="HazardRatio" dataDxfId="41"/>
-    <tableColumn id="9" name="RobustWaldLower" dataDxfId="44"/>
-    <tableColumn id="10" name="RobustWaldUpper" dataDxfId="43"/>
+    <tableColumn id="6" name="nTNF" dataDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="nComparator" dataDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="HazardRatio" dataDxfId="2"/>
+    <tableColumn id="9" name="RobustWaldLower" dataDxfId="1"/>
+    <tableColumn id="10" name="RobustWaldUpper" dataDxfId="0"/>
     <tableColumn id="11" name="indValidHR"/>
     <tableColumn id="12" name="indSigHR"/>
   </tableColumns>
@@ -4674,7 +4674,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="A1:F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4918,8 +4920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5357,13 +5359,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.140625" style="2" bestFit="1" customWidth="1"/>
@@ -7242,14 +7246,14 @@
   <dimension ref="A1:O93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="O90" sqref="A1:O90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="2" bestFit="1" customWidth="1"/>

</xml_diff>